<commit_message>
Backup QR Scanner data - 26/07/2025, 10:36:25 PM
</commit_message>
<xml_diff>
--- a/log_history/Y1_B2425_all_sessions.xlsx
+++ b/log_history/Y1_B2425_all_sessions.xlsx
@@ -4,8 +4,6 @@
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="Anatomy" sheetId="1" r:id="rId1"/>
-    <sheet name="Anatomy_2" sheetId="2" r:id="rId2"/>
-    <sheet name="Anatomy_3" sheetId="3" r:id="rId3"/>
   </sheets>
 </workbook>
 </file>
@@ -426,124 +424,16 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>228722</v>
+        <v>424333</v>
       </c>
       <c r="B2" t="str">
         <v>Anatomy</v>
       </c>
       <c r="C2" t="str">
-        <v>25/07/2025</v>
+        <v>26/07/2025</v>
       </c>
       <c r="D2" t="str">
-        <v>12:32:17</v>
-      </c>
-      <c r="E2" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F2" t="str">
-        <v>231249@med.asu.edu.eg</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F2"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Student ID</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Subject</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Log Date</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Log Time</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Type</v>
-      </c>
-      <c r="F1" t="str">
-        <v>User</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>812282</v>
-      </c>
-      <c r="B2" t="str">
-        <v>Anatomy</v>
-      </c>
-      <c r="C2" t="str">
-        <v>26/07/2025</v>
-      </c>
-      <c r="D2" t="str">
-        <v>03:31:10</v>
-      </c>
-      <c r="E2" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F2" t="str">
-        <v>231249@med.asu.edu.eg</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F2"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Student ID</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Subject</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Log Date</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Log Time</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Type</v>
-      </c>
-      <c r="F1" t="str">
-        <v>User</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>558525</v>
-      </c>
-      <c r="B2" t="str">
-        <v>Anatomy</v>
-      </c>
-      <c r="C2" t="str">
-        <v>26/07/2025</v>
-      </c>
-      <c r="D2" t="str">
-        <v>03:34:36</v>
+        <v>22:35:50</v>
       </c>
       <c r="E2" t="str">
         <v>Manual</v>

</xml_diff>